<commit_message>
Altium sources, converted from Xpedition
</commit_message>
<xml_diff>
--- a/PCB_AFCZ/Output/AFCZ.xlsx
+++ b/PCB_AFCZ/Output/AFCZ.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1049" uniqueCount="713">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1047" uniqueCount="708">
   <si>
     <t>#</t>
   </si>
@@ -155,7 +155,7 @@
     <t>Capacitor - non polarized CAPC1005X55N</t>
   </si>
   <si>
-    <t>C232,C367,C444,C497,C508</t>
+    <t>C232,C367,C444,C497,C508,C989</t>
   </si>
   <si>
     <t>CAPC1005X55N</t>
@@ -452,7 +452,7 @@
     <t>Medium Power AF Schottky Diode</t>
   </si>
   <si>
-    <t>D1-D6,D29-D33</t>
+    <t>D1-D6,D29-D34</t>
   </si>
   <si>
     <t>SOD2512X110N</t>
@@ -593,21 +593,6 @@
     <t>Aavid Thermalloy</t>
   </si>
   <si>
-    <t>M25P128-VME6G</t>
-  </si>
-  <si>
-    <t>128 Mbit (Multilevel), Low-Voltage, Serial Flash Memory With 50-MHz SPI Bus Interface</t>
-  </si>
-  <si>
-    <t>IC1</t>
-  </si>
-  <si>
-    <t>PSON127P800X600X100-9N-R640X480</t>
-  </si>
-  <si>
-    <t>NUMONYX</t>
-  </si>
-  <si>
     <t>SN74CB3T3257PW</t>
   </si>
   <si>
@@ -824,15 +809,15 @@
     <t>MARVELL</t>
   </si>
   <si>
-    <t>AT24C01BN-SH-B</t>
-  </si>
-  <si>
-    <t>1.8V to 5.5V, 1K (128 x 8), 2-Wire Bus Serial EEPROM With Full Memory Write Protect</t>
+    <t>SCANSTA112VS/NOPB</t>
   </si>
   <si>
     <t>IC24</t>
   </si>
   <si>
+    <t>QFP50P1600X1600X120-100N</t>
+  </si>
+  <si>
     <t>TCA9548ARGER</t>
   </si>
   <si>
@@ -1073,6 +1058,15 @@
     <t>QFN50P600X600X90-37N-S425</t>
   </si>
   <si>
+    <t>24LC024H-I/SN</t>
+  </si>
+  <si>
+    <t>2.5V-5.5V, 2K (256 x 8-bit) I2C Serial EEPROM With Half-Array Write Protect</t>
+  </si>
+  <si>
+    <t>IC66</t>
+  </si>
+  <si>
     <t>TPS74801DRCT</t>
   </si>
   <si>
@@ -1094,6 +1088,21 @@
     <t>SOT95P237X112-3N</t>
   </si>
   <si>
+    <t>W25Q128JVSIM</t>
+  </si>
+  <si>
+    <t>3V  128 M - BIT SERIAL FLASH MEMORY  WITH  DUAL / QUAD SPI &amp; QPI &amp; DTR</t>
+  </si>
+  <si>
+    <t>IC76</t>
+  </si>
+  <si>
+    <t>SOIC127P790X216-8N</t>
+  </si>
+  <si>
+    <t>Winbond</t>
+  </si>
+  <si>
     <t>SAMTEC_FTS-105-02-F-DV</t>
   </si>
   <si>
@@ -1235,7 +1244,7 @@
     <t>120R@100MHz</t>
   </si>
   <si>
-    <t>L1-L8,L57,L58,L80,L83</t>
+    <t>L1-L8,L80,L83</t>
   </si>
   <si>
     <t>INDC1608X95N</t>
@@ -1343,7 +1352,7 @@
     <t>60R@100MHz</t>
   </si>
   <si>
-    <t>L37-L39,L41-L43,L78,L84</t>
+    <t>L37-L39,L41-L43,L78,L84-L92</t>
   </si>
   <si>
     <t>INDC4516X180N</t>
@@ -1484,24 +1493,15 @@
     <t>IQD FREQUENCY PRODUCTS</t>
   </si>
   <si>
-    <t>OSC_20MHZ_IQD_LF VCXO026156</t>
-  </si>
-  <si>
-    <t>3.3V ±100ppm 15pF HCMOS Tri-State Surface Mount Voltage Controlled Oscillator VCXO (CFPV-45 Series)</t>
-  </si>
-  <si>
-    <t>20MHz</t>
+    <t>OSC_20MHZ_KYOCERA_KV7050B20.0000C3GD00</t>
+  </si>
+  <si>
+    <t>Voltage Controlled Crystal Oscillators (VCXO)  Surface Mount Type   KV7050B-C3 Series</t>
   </si>
   <si>
     <t>OSC2,OSC3</t>
   </si>
   <si>
-    <t>OSC_IQD_CFPV-45</t>
-  </si>
-  <si>
-    <t>LF VCXO026156</t>
-  </si>
-  <si>
     <t>SW_C&amp;K_HDT0001</t>
   </si>
   <si>
@@ -1667,7 +1667,7 @@
     <t>1A (0.05R Max DC Resistance) Zero Ohm Jumper,General Purpose Thick Film Chip Resistor</t>
   </si>
   <si>
-    <t>R1-R4,R7,R45,R46,R60,R63,R67,R68,R70-R74,R79-R82,R94,R111,R113-R119,R137-R140,R147,R157,R270-R272,R279-R281,R289,R308,R309,R396-R399,R469,R471-R473,R495,R496,R511,R514-R517,R519,R520,R524,R528,R529,R531,R532,R537,R538,R549-R552,R555,R558,R561-R566,R587,R591,R594,R595,R604-R607,R616,R626,R646-R649</t>
+    <t>R1-R4,R45,R46,R60,R63,R67,R68,R70-R74,R79-R82,R94,R111,R113-R119,R137-R140,R147,R157,R270-R272,R279-R281,R289,R308,R309,R396-R399,R469,R471-R473,R495,R496,R511,R514-R517,R519,R520,R524,R528,R529,R531,R532,R537,R538,R549-R552,R555,R558,R561-R566,R587,R591,R594,R595,R604-R607,R616,R626,R646-R649</t>
   </si>
   <si>
     <t>R0402_0R_JUMPER,R0402_2K2_1%_0.0625W_100PPM</t>
@@ -1688,16 +1688,28 @@
     <t>1k</t>
   </si>
   <si>
-    <t>R6,R172,R247,R304,R342,R343,R352,R400,R433,R449-R452,R459,R512,R576,R586,R592,R603,R608,R613,R617</t>
+    <t>R6,R172,R247,R304,R342,R343,R352,R400,R433,R449-R452,R459,R512,R576,R586,R592,R603,R608,R613,R617,R651,R652</t>
   </si>
   <si>
     <t>R0402_1K_1%_0.0625W_100PPM</t>
   </si>
   <si>
+    <t>1A (0.05R Max DC Resistance) Zero Ohm Jumper,General Purpose Thick Film Chip Resistor,Reserved Footprint For a 0402 (1005) Chip Resistor</t>
+  </si>
+  <si>
+    <t>R7,R37-R40,R78,R83,R89-R93,R109,R148,R154-R156,R192,R193</t>
+  </si>
+  <si>
+    <t>R0402_0R_JUMPER,R0402_2K2_1%_0.0625W_100PPM,R0402_NO-VALUE</t>
+  </si>
+  <si>
+    <t>GENERIC,Undefined</t>
+  </si>
+  <si>
     <t>10k</t>
   </si>
   <si>
-    <t>R8,R24-R36,R41,R42,R44,R49,R50,R52-R57,R61,R62,R64-R66,R69,R75-R77,R84-R88,R95-R108,R110,R112,R120,R121,R131,R133-R135,R141-R146,R149-R153,R158,R160-R165,R168,R173-R175,R287,R297-R301,R351,R387,R390,R391,R393,R401,R454,R455,R466,R467,R470,R501,R502,R505,R508,R510,R513,R554,R559,R574,R575,R581-R583,R588-R590,R596-R602,R609-R612,R614,R618,R622,R625,R627,R628,R633,R635,R637-R640,R645</t>
+    <t>R8,R24-R36,R41,R42,R44,R49,R50,R52-R57,R61,R62,R64-R66,R69,R75-R77,R84-R88,R95-R108,R110,R112,R120,R121,R131,R133-R135,R141-R146,R149-R153,R158,R160-R165,R168,R173-R175,R287,R297-R301,R351,R387,R390,R391,R393,R401,R454,R455,R466,R467,R470,R501,R502,R505,R508,R510,R513,R554,R559,R574,R575,R581-R583,R588-R590,R596-R602,R609-R612,R614,R618,R622,R625,R627,R628,R633,R635,R637-R640,R645,R653</t>
   </si>
   <si>
     <t>RESC1005X40N</t>
@@ -1727,18 +1739,6 @@
     <t>R0402_2K2_1%_0.0625W_100PPM</t>
   </si>
   <si>
-    <t>1A (0.05R Max DC Resistance) Zero Ohm Jumper,General Purpose Thick Film Chip Resistor,Reserved Footprint For a 0402 (1005) Chip Resistor</t>
-  </si>
-  <si>
-    <t>R37-R40,R78,R83,R89-R93,R109,R148,R154-R156,R192,R193</t>
-  </si>
-  <si>
-    <t>R0402_0R_JUMPER,R0402_2K2_1%_0.0625W_100PPM,R0402_NO-VALUE</t>
-  </si>
-  <si>
-    <t>GENERIC,Undefined</t>
-  </si>
-  <si>
     <t>12k</t>
   </si>
   <si>
@@ -1907,21 +1907,6 @@
     <t>VISHAY DALE</t>
   </si>
   <si>
-    <t>Resistor - 1% RESC5226X80N</t>
-  </si>
-  <si>
-    <t>Low Value Flat Chip Resistor</t>
-  </si>
-  <si>
-    <t>R367</t>
-  </si>
-  <si>
-    <t>LRF2010-R02FW</t>
-  </si>
-  <si>
-    <t>WELWYN COMPONENTS</t>
-  </si>
-  <si>
     <t>Resistor - 1% RESC0603X28N</t>
   </si>
   <si>
@@ -1964,7 +1949,7 @@
     <t>16A (0.005R Max DC Resistance) Zero Ohm Jumper</t>
   </si>
   <si>
-    <t>R518,R527</t>
+    <t>R518,R527,R650</t>
   </si>
   <si>
     <t>R2512_0R_JUMPER</t>
@@ -1988,13 +1973,25 @@
     <t>R0402_16K_1%_0.0625W_100PPM</t>
   </si>
   <si>
+    <t>Resistor - 1% RESC6532X80N</t>
+  </si>
+  <si>
+    <t>0R5</t>
+  </si>
+  <si>
+    <t>R654</t>
+  </si>
+  <si>
+    <t>R2512_0R5_1%_1.5W_100PPM</t>
+  </si>
+  <si>
     <t>SW_TYCO_1571983-4</t>
   </si>
   <si>
     <t>4 Way SPST SMD DIP Switch, Latched, Contact Rating 0.025A 24VDC</t>
   </si>
   <si>
-    <t>SW1</t>
+    <t>SW1,SW2</t>
   </si>
   <si>
     <t>1571983-4 or GDH04S04</t>
@@ -2003,18 +2000,6 @@
     <t>TYCO</t>
   </si>
   <si>
-    <t>SW_TYCO_1571983-1</t>
-  </si>
-  <si>
-    <t>2 Way SPST SMD DIP Switch, Latched, Contact Rating 0.025A 24VDC</t>
-  </si>
-  <si>
-    <t>SW2,SW3</t>
-  </si>
-  <si>
-    <t>1571983-1 or GDH02S04</t>
-  </si>
-  <si>
     <t>BSS138LT1G</t>
   </si>
   <si>
@@ -2060,7 +2045,7 @@
     <t>-30V -19.7A P-Channel MOSFET</t>
   </si>
   <si>
-    <t>T11-T13,T29</t>
+    <t>T11-T13,T29,T40</t>
   </si>
   <si>
     <t>BC857BV</t>
@@ -2762,7 +2747,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C11" t="s">
         <v>42</v>
@@ -3545,7 +3530,7 @@
         <v>37</v>
       </c>
       <c r="B38">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C38" t="s">
         <v>140</v>
@@ -3793,7 +3778,7 @@
         <v>47</v>
       </c>
       <c r="B48">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C48" t="s">
         <v>189</v>
@@ -3819,7 +3804,7 @@
         <v>48</v>
       </c>
       <c r="B49">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C49" t="s">
         <v>194</v>
@@ -3837,7 +3822,7 @@
         <v>194</v>
       </c>
       <c r="I49" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
@@ -3845,25 +3830,25 @@
         <v>49</v>
       </c>
       <c r="B50">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C50" t="s">
+        <v>198</v>
+      </c>
+      <c r="D50" t="s">
         <v>199</v>
       </c>
-      <c r="D50" t="s">
+      <c r="F50" t="s">
         <v>200</v>
       </c>
-      <c r="F50" t="s">
+      <c r="G50" t="s">
         <v>201</v>
       </c>
-      <c r="G50" t="s">
-        <v>202</v>
-      </c>
       <c r="H50" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="I50" t="s">
-        <v>198</v>
+        <v>149</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
@@ -3871,25 +3856,25 @@
         <v>50</v>
       </c>
       <c r="B51">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C51" t="s">
+        <v>202</v>
+      </c>
+      <c r="D51" t="s">
         <v>203</v>
       </c>
-      <c r="D51" t="s">
+      <c r="F51" t="s">
         <v>204</v>
       </c>
-      <c r="F51" t="s">
+      <c r="G51" t="s">
         <v>205</v>
       </c>
-      <c r="G51" t="s">
-        <v>206</v>
-      </c>
       <c r="H51" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I51" t="s">
-        <v>149</v>
+        <v>193</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
@@ -3897,25 +3882,25 @@
         <v>51</v>
       </c>
       <c r="B52">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C52" t="s">
+        <v>206</v>
+      </c>
+      <c r="D52" t="s">
         <v>207</v>
       </c>
-      <c r="D52" t="s">
+      <c r="F52" t="s">
         <v>208</v>
       </c>
-      <c r="F52" t="s">
+      <c r="G52" t="s">
         <v>209</v>
       </c>
-      <c r="G52" t="s">
-        <v>210</v>
-      </c>
       <c r="H52" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I52" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
@@ -3923,25 +3908,25 @@
         <v>52</v>
       </c>
       <c r="B53">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C53" t="s">
+        <v>210</v>
+      </c>
+      <c r="D53" t="s">
         <v>211</v>
       </c>
-      <c r="D53" t="s">
+      <c r="F53" t="s">
         <v>212</v>
       </c>
-      <c r="F53" t="s">
+      <c r="G53" t="s">
         <v>213</v>
       </c>
-      <c r="G53" t="s">
+      <c r="H53" t="s">
+        <v>210</v>
+      </c>
+      <c r="I53" t="s">
         <v>214</v>
-      </c>
-      <c r="H53" t="s">
-        <v>211</v>
-      </c>
-      <c r="I53" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
@@ -3983,6 +3968,9 @@
       <c r="D55" t="s">
         <v>221</v>
       </c>
+      <c r="E55" t="s">
+        <v>34</v>
+      </c>
       <c r="F55" t="s">
         <v>222</v>
       </c>
@@ -4001,7 +3989,7 @@
         <v>55</v>
       </c>
       <c r="B56">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C56" t="s">
         <v>225</v>
@@ -4019,7 +4007,7 @@
         <v>225</v>
       </c>
       <c r="I56" t="s">
-        <v>229</v>
+        <v>193</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
@@ -4027,25 +4015,25 @@
         <v>56</v>
       </c>
       <c r="B57">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C57" t="s">
+        <v>229</v>
+      </c>
+      <c r="D57" t="s">
         <v>230</v>
       </c>
-      <c r="D57" t="s">
+      <c r="F57" t="s">
         <v>231</v>
       </c>
-      <c r="F57" t="s">
+      <c r="G57" t="s">
         <v>232</v>
       </c>
-      <c r="G57" t="s">
+      <c r="H57" t="s">
+        <v>229</v>
+      </c>
+      <c r="I57" t="s">
         <v>233</v>
-      </c>
-      <c r="H57" t="s">
-        <v>230</v>
-      </c>
-      <c r="I57" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
@@ -4053,7 +4041,7 @@
         <v>57</v>
       </c>
       <c r="B58">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C58" t="s">
         <v>234</v>
@@ -4071,7 +4059,7 @@
         <v>234</v>
       </c>
       <c r="I58" t="s">
-        <v>238</v>
+        <v>149</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
@@ -4079,25 +4067,25 @@
         <v>58</v>
       </c>
       <c r="B59">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C59" t="s">
+        <v>238</v>
+      </c>
+      <c r="D59" t="s">
         <v>239</v>
       </c>
-      <c r="D59" t="s">
+      <c r="F59" t="s">
         <v>240</v>
       </c>
-      <c r="F59" t="s">
+      <c r="G59" t="s">
         <v>241</v>
       </c>
-      <c r="G59" t="s">
-        <v>242</v>
-      </c>
       <c r="H59" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I59" t="s">
-        <v>149</v>
+        <v>193</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
@@ -4105,25 +4093,25 @@
         <v>59</v>
       </c>
       <c r="B60">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C60" t="s">
+        <v>242</v>
+      </c>
+      <c r="D60" t="s">
         <v>243</v>
       </c>
-      <c r="D60" t="s">
+      <c r="F60" t="s">
         <v>244</v>
       </c>
-      <c r="F60" t="s">
+      <c r="G60" t="s">
         <v>245</v>
       </c>
-      <c r="G60" t="s">
+      <c r="H60" t="s">
+        <v>242</v>
+      </c>
+      <c r="I60" t="s">
         <v>246</v>
-      </c>
-      <c r="H60" t="s">
-        <v>243</v>
-      </c>
-      <c r="I60" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
@@ -4149,7 +4137,7 @@
         <v>247</v>
       </c>
       <c r="I61" t="s">
-        <v>251</v>
+        <v>193</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
@@ -4157,25 +4145,25 @@
         <v>61</v>
       </c>
       <c r="B62">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C62" t="s">
+        <v>251</v>
+      </c>
+      <c r="D62" t="s">
         <v>252</v>
       </c>
-      <c r="D62" t="s">
+      <c r="F62" t="s">
         <v>253</v>
       </c>
-      <c r="F62" t="s">
+      <c r="G62" t="s">
         <v>254</v>
       </c>
-      <c r="G62" t="s">
+      <c r="H62" t="s">
+        <v>251</v>
+      </c>
+      <c r="I62" t="s">
         <v>255</v>
-      </c>
-      <c r="H62" t="s">
-        <v>252</v>
-      </c>
-      <c r="I62" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
@@ -4183,9 +4171,9 @@
         <v>62</v>
       </c>
       <c r="B63">
-        <v>10</v>
-      </c>
-      <c r="C63" t="s">
+        <v>1</v>
+      </c>
+      <c r="C63" s="1" t="s">
         <v>256</v>
       </c>
       <c r="D63" t="s">
@@ -4197,7 +4185,7 @@
       <c r="G63" t="s">
         <v>259</v>
       </c>
-      <c r="H63" t="s">
+      <c r="H63" s="1" t="s">
         <v>256</v>
       </c>
       <c r="I63" t="s">
@@ -4211,23 +4199,23 @@
       <c r="B64">
         <v>1</v>
       </c>
-      <c r="C64" s="1" t="s">
+      <c r="C64" t="s">
         <v>261</v>
       </c>
       <c r="D64" t="s">
+        <v>221</v>
+      </c>
+      <c r="F64" t="s">
         <v>262</v>
       </c>
-      <c r="F64" t="s">
+      <c r="G64" t="s">
         <v>263</v>
       </c>
-      <c r="G64" t="s">
-        <v>264</v>
-      </c>
-      <c r="H64" s="1" t="s">
+      <c r="H64" t="s">
         <v>261</v>
       </c>
       <c r="I64" t="s">
-        <v>265</v>
+        <v>193</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
@@ -4235,25 +4223,25 @@
         <v>64</v>
       </c>
       <c r="B65">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C65" t="s">
+        <v>264</v>
+      </c>
+      <c r="D65" t="s">
+        <v>265</v>
+      </c>
+      <c r="F65" t="s">
         <v>266</v>
       </c>
-      <c r="D65" t="s">
+      <c r="G65" t="s">
         <v>267</v>
       </c>
-      <c r="F65" t="s">
-        <v>268</v>
-      </c>
-      <c r="G65" t="s">
-        <v>250</v>
-      </c>
       <c r="H65" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="I65" t="s">
-        <v>219</v>
+        <v>193</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
@@ -4261,25 +4249,25 @@
         <v>65</v>
       </c>
       <c r="B66">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C66" t="s">
+        <v>268</v>
+      </c>
+      <c r="D66" t="s">
         <v>269</v>
       </c>
-      <c r="D66" t="s">
+      <c r="F66" t="s">
         <v>270</v>
       </c>
-      <c r="F66" t="s">
+      <c r="G66" t="s">
         <v>271</v>
       </c>
-      <c r="G66" t="s">
+      <c r="H66" t="s">
+        <v>268</v>
+      </c>
+      <c r="I66" t="s">
         <v>272</v>
-      </c>
-      <c r="H66" t="s">
-        <v>269</v>
-      </c>
-      <c r="I66" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
@@ -4287,7 +4275,7 @@
         <v>66</v>
       </c>
       <c r="B67">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C67" t="s">
         <v>273</v>
@@ -4305,7 +4293,7 @@
         <v>273</v>
       </c>
       <c r="I67" t="s">
-        <v>277</v>
+        <v>193</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
@@ -4313,25 +4301,25 @@
         <v>67</v>
       </c>
       <c r="B68">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C68" t="s">
+        <v>277</v>
+      </c>
+      <c r="D68" t="s">
         <v>278</v>
       </c>
-      <c r="D68" t="s">
+      <c r="F68" t="s">
         <v>279</v>
       </c>
-      <c r="F68" t="s">
+      <c r="G68" t="s">
         <v>280</v>
       </c>
-      <c r="G68" t="s">
+      <c r="H68" t="s">
+        <v>277</v>
+      </c>
+      <c r="I68" t="s">
         <v>281</v>
-      </c>
-      <c r="H68" t="s">
-        <v>278</v>
-      </c>
-      <c r="I68" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
@@ -4365,7 +4353,7 @@
         <v>69</v>
       </c>
       <c r="B70">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C70" t="s">
         <v>287</v>
@@ -4391,7 +4379,7 @@
         <v>70</v>
       </c>
       <c r="B71">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C71" t="s">
         <v>292</v>
@@ -4435,7 +4423,7 @@
         <v>297</v>
       </c>
       <c r="I72" t="s">
-        <v>301</v>
+        <v>193</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
@@ -4443,25 +4431,25 @@
         <v>72</v>
       </c>
       <c r="B73">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C73" t="s">
+        <v>301</v>
+      </c>
+      <c r="D73" t="s">
         <v>302</v>
       </c>
-      <c r="D73" t="s">
+      <c r="F73" t="s">
         <v>303</v>
       </c>
-      <c r="F73" t="s">
+      <c r="G73" t="s">
         <v>304</v>
       </c>
-      <c r="G73" t="s">
-        <v>305</v>
-      </c>
       <c r="H73" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="I73" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
@@ -4472,22 +4460,22 @@
         <v>1</v>
       </c>
       <c r="C74" t="s">
+        <v>305</v>
+      </c>
+      <c r="D74" t="s">
         <v>306</v>
       </c>
-      <c r="D74" t="s">
+      <c r="F74" t="s">
         <v>307</v>
       </c>
-      <c r="F74" t="s">
+      <c r="G74" t="s">
         <v>308</v>
       </c>
-      <c r="G74" t="s">
-        <v>309</v>
-      </c>
       <c r="H74" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="I74" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
@@ -4498,22 +4486,22 @@
         <v>1</v>
       </c>
       <c r="C75" t="s">
+        <v>309</v>
+      </c>
+      <c r="D75" t="s">
         <v>310</v>
       </c>
-      <c r="D75" t="s">
+      <c r="F75" t="s">
         <v>311</v>
       </c>
-      <c r="F75" t="s">
+      <c r="G75" t="s">
         <v>312</v>
       </c>
-      <c r="G75" t="s">
+      <c r="H75" t="s">
+        <v>309</v>
+      </c>
+      <c r="I75" t="s">
         <v>313</v>
-      </c>
-      <c r="H75" t="s">
-        <v>310</v>
-      </c>
-      <c r="I75" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
@@ -4533,13 +4521,13 @@
         <v>316</v>
       </c>
       <c r="G76" t="s">
-        <v>317</v>
+        <v>304</v>
       </c>
       <c r="H76" t="s">
         <v>314</v>
       </c>
       <c r="I76" t="s">
-        <v>318</v>
+        <v>193</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
@@ -4550,22 +4538,22 @@
         <v>1</v>
       </c>
       <c r="C77" t="s">
+        <v>317</v>
+      </c>
+      <c r="D77" t="s">
+        <v>318</v>
+      </c>
+      <c r="F77" t="s">
         <v>319</v>
       </c>
-      <c r="D77" t="s">
+      <c r="G77" t="s">
         <v>320</v>
       </c>
-      <c r="F77" t="s">
+      <c r="H77" t="s">
+        <v>317</v>
+      </c>
+      <c r="I77" t="s">
         <v>321</v>
-      </c>
-      <c r="G77" t="s">
-        <v>309</v>
-      </c>
-      <c r="H77" t="s">
-        <v>319</v>
-      </c>
-      <c r="I77" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
@@ -4585,13 +4573,13 @@
         <v>324</v>
       </c>
       <c r="G78" t="s">
-        <v>325</v>
+        <v>245</v>
       </c>
       <c r="H78" t="s">
         <v>322</v>
       </c>
       <c r="I78" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
@@ -4602,19 +4590,19 @@
         <v>1</v>
       </c>
       <c r="C79" t="s">
+        <v>326</v>
+      </c>
+      <c r="D79" t="s">
         <v>327</v>
       </c>
-      <c r="D79" t="s">
+      <c r="E79" t="s">
+        <v>326</v>
+      </c>
+      <c r="F79" t="s">
         <v>328</v>
       </c>
-      <c r="F79" t="s">
+      <c r="G79" t="s">
         <v>329</v>
-      </c>
-      <c r="G79" t="s">
-        <v>250</v>
-      </c>
-      <c r="H79" t="s">
-        <v>327</v>
       </c>
       <c r="I79" t="s">
         <v>330</v>
@@ -4625,7 +4613,7 @@
         <v>79</v>
       </c>
       <c r="B80">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C80" t="s">
         <v>331</v>
@@ -4633,14 +4621,14 @@
       <c r="D80" t="s">
         <v>332</v>
       </c>
-      <c r="E80" t="s">
-        <v>331</v>
-      </c>
       <c r="F80" t="s">
         <v>333</v>
       </c>
       <c r="G80" t="s">
         <v>334</v>
+      </c>
+      <c r="H80" t="s">
+        <v>331</v>
       </c>
       <c r="I80" t="s">
         <v>335</v>
@@ -4651,7 +4639,7 @@
         <v>80</v>
       </c>
       <c r="B81">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C81" t="s">
         <v>336</v>
@@ -4659,6 +4647,9 @@
       <c r="D81" t="s">
         <v>337</v>
       </c>
+      <c r="E81" t="s">
+        <v>34</v>
+      </c>
       <c r="F81" t="s">
         <v>338</v>
       </c>
@@ -4669,7 +4660,7 @@
         <v>336</v>
       </c>
       <c r="I81" t="s">
-        <v>340</v>
+        <v>149</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
@@ -4680,25 +4671,22 @@
         <v>1</v>
       </c>
       <c r="C82" t="s">
+        <v>340</v>
+      </c>
+      <c r="D82" t="s">
         <v>341</v>
       </c>
-      <c r="D82" t="s">
+      <c r="F82" t="s">
         <v>342</v>
       </c>
-      <c r="E82" t="s">
-        <v>34</v>
-      </c>
-      <c r="F82" t="s">
+      <c r="G82" t="s">
         <v>343</v>
       </c>
-      <c r="G82" t="s">
-        <v>344</v>
-      </c>
       <c r="H82" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="I82" t="s">
-        <v>149</v>
+        <v>321</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
@@ -4709,22 +4697,22 @@
         <v>1</v>
       </c>
       <c r="C83" t="s">
+        <v>344</v>
+      </c>
+      <c r="D83" t="s">
         <v>345</v>
       </c>
-      <c r="D83" t="s">
+      <c r="F83" t="s">
         <v>346</v>
       </c>
-      <c r="F83" t="s">
-        <v>347</v>
-      </c>
       <c r="G83" t="s">
-        <v>348</v>
+        <v>245</v>
       </c>
       <c r="H83" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="I83" t="s">
-        <v>326</v>
+        <v>272</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
@@ -4735,22 +4723,22 @@
         <v>2</v>
       </c>
       <c r="C84" t="s">
+        <v>347</v>
+      </c>
+      <c r="D84" t="s">
+        <v>348</v>
+      </c>
+      <c r="F84" t="s">
         <v>349</v>
       </c>
-      <c r="D84" t="s">
-        <v>350</v>
-      </c>
-      <c r="F84" t="s">
-        <v>351</v>
-      </c>
       <c r="G84" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="H84" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="I84" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
@@ -4761,22 +4749,22 @@
         <v>1</v>
       </c>
       <c r="C85" t="s">
+        <v>350</v>
+      </c>
+      <c r="D85" t="s">
+        <v>351</v>
+      </c>
+      <c r="F85" t="s">
         <v>352</v>
       </c>
-      <c r="D85" t="s">
+      <c r="G85" t="s">
         <v>353</v>
       </c>
-      <c r="F85" t="s">
-        <v>354</v>
-      </c>
-      <c r="G85" t="s">
-        <v>355</v>
-      </c>
       <c r="H85" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="I85" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
@@ -4787,22 +4775,22 @@
         <v>1</v>
       </c>
       <c r="C86" t="s">
+        <v>354</v>
+      </c>
+      <c r="D86" t="s">
+        <v>355</v>
+      </c>
+      <c r="F86" t="s">
         <v>356</v>
       </c>
-      <c r="D86" t="s">
+      <c r="G86" t="s">
         <v>357</v>
       </c>
-      <c r="F86" t="s">
+      <c r="H86" t="s">
+        <v>354</v>
+      </c>
+      <c r="I86" t="s">
         <v>358</v>
-      </c>
-      <c r="G86" t="s">
-        <v>356</v>
-      </c>
-      <c r="H86" t="s">
-        <v>359</v>
-      </c>
-      <c r="I86" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
@@ -4810,25 +4798,25 @@
         <v>86</v>
       </c>
       <c r="B87">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C87" t="s">
+        <v>359</v>
+      </c>
+      <c r="D87" t="s">
+        <v>360</v>
+      </c>
+      <c r="F87" t="s">
         <v>361</v>
       </c>
-      <c r="D87" t="s">
+      <c r="G87" t="s">
+        <v>359</v>
+      </c>
+      <c r="H87" t="s">
         <v>362</v>
       </c>
-      <c r="F87" t="s">
+      <c r="I87" t="s">
         <v>363</v>
-      </c>
-      <c r="G87" t="s">
-        <v>361</v>
-      </c>
-      <c r="H87" t="s">
-        <v>364</v>
-      </c>
-      <c r="I87" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
@@ -4836,25 +4824,25 @@
         <v>87</v>
       </c>
       <c r="B88">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C88" t="s">
+        <v>364</v>
+      </c>
+      <c r="D88" t="s">
+        <v>365</v>
+      </c>
+      <c r="F88" t="s">
         <v>366</v>
       </c>
-      <c r="D88" t="s">
+      <c r="G88" t="s">
+        <v>364</v>
+      </c>
+      <c r="H88" t="s">
         <v>367</v>
       </c>
-      <c r="F88" t="s">
+      <c r="I88" t="s">
         <v>368</v>
-      </c>
-      <c r="G88" t="s">
-        <v>366</v>
-      </c>
-      <c r="H88" t="s">
-        <v>369</v>
-      </c>
-      <c r="I88" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
@@ -4865,19 +4853,22 @@
         <v>1</v>
       </c>
       <c r="C89" t="s">
+        <v>369</v>
+      </c>
+      <c r="D89" t="s">
         <v>370</v>
       </c>
-      <c r="D89" t="s">
+      <c r="F89" t="s">
         <v>371</v>
       </c>
-      <c r="F89" t="s">
+      <c r="G89" t="s">
+        <v>369</v>
+      </c>
+      <c r="H89" t="s">
         <v>372</v>
       </c>
-      <c r="H89" t="s">
-        <v>373</v>
-      </c>
       <c r="I89" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
@@ -4885,25 +4876,22 @@
         <v>89</v>
       </c>
       <c r="B90">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C90" t="s">
+        <v>373</v>
+      </c>
+      <c r="D90" t="s">
         <v>374</v>
       </c>
-      <c r="D90" t="s">
+      <c r="F90" t="s">
         <v>375</v>
       </c>
-      <c r="F90" t="s">
+      <c r="H90" t="s">
         <v>376</v>
       </c>
-      <c r="G90" t="s">
-        <v>374</v>
-      </c>
-      <c r="H90" t="s">
-        <v>377</v>
-      </c>
       <c r="I90" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
@@ -4911,25 +4899,25 @@
         <v>90</v>
       </c>
       <c r="B91">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C91" t="s">
+        <v>377</v>
+      </c>
+      <c r="D91" t="s">
+        <v>378</v>
+      </c>
+      <c r="F91" t="s">
         <v>379</v>
       </c>
-      <c r="D91" t="s">
+      <c r="G91" t="s">
+        <v>377</v>
+      </c>
+      <c r="H91" t="s">
         <v>380</v>
       </c>
-      <c r="F91" t="s">
+      <c r="I91" t="s">
         <v>381</v>
-      </c>
-      <c r="G91" t="s">
-        <v>379</v>
-      </c>
-      <c r="H91" t="s">
-        <v>382</v>
-      </c>
-      <c r="I91" t="s">
-        <v>383</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
@@ -4940,22 +4928,22 @@
         <v>1</v>
       </c>
       <c r="C92" t="s">
+        <v>382</v>
+      </c>
+      <c r="D92" t="s">
+        <v>383</v>
+      </c>
+      <c r="F92" t="s">
         <v>384</v>
       </c>
-      <c r="D92" t="s">
+      <c r="G92" t="s">
+        <v>382</v>
+      </c>
+      <c r="H92" t="s">
         <v>385</v>
       </c>
-      <c r="F92" t="s">
+      <c r="I92" t="s">
         <v>386</v>
-      </c>
-      <c r="G92" t="s">
-        <v>384</v>
-      </c>
-      <c r="H92" t="s">
-        <v>387</v>
-      </c>
-      <c r="I92" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
@@ -4966,22 +4954,22 @@
         <v>1</v>
       </c>
       <c r="C93" t="s">
+        <v>387</v>
+      </c>
+      <c r="D93" t="s">
         <v>388</v>
       </c>
-      <c r="D93" t="s">
+      <c r="F93" t="s">
         <v>389</v>
       </c>
-      <c r="F93" t="s">
+      <c r="G93" t="s">
+        <v>387</v>
+      </c>
+      <c r="H93" t="s">
         <v>390</v>
       </c>
-      <c r="G93" t="s">
-        <v>388</v>
-      </c>
-      <c r="H93" t="s">
-        <v>391</v>
-      </c>
       <c r="I93" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
@@ -4992,22 +4980,22 @@
         <v>1</v>
       </c>
       <c r="C94" t="s">
+        <v>391</v>
+      </c>
+      <c r="D94" t="s">
         <v>392</v>
       </c>
-      <c r="D94" t="s">
+      <c r="F94" t="s">
         <v>393</v>
       </c>
-      <c r="F94" t="s">
+      <c r="G94" t="s">
+        <v>391</v>
+      </c>
+      <c r="H94" t="s">
         <v>394</v>
       </c>
-      <c r="G94" t="s">
-        <v>392</v>
-      </c>
-      <c r="H94">
-        <v>692622030100</v>
-      </c>
       <c r="I94" t="s">
-        <v>395</v>
+        <v>381</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
@@ -5018,22 +5006,22 @@
         <v>1</v>
       </c>
       <c r="C95" t="s">
+        <v>395</v>
+      </c>
+      <c r="D95" t="s">
         <v>396</v>
       </c>
-      <c r="D95" t="s">
+      <c r="F95" t="s">
         <v>397</v>
       </c>
-      <c r="F95" t="s">
+      <c r="G95" t="s">
+        <v>395</v>
+      </c>
+      <c r="H95">
+        <v>692622030100</v>
+      </c>
+      <c r="I95" t="s">
         <v>398</v>
-      </c>
-      <c r="G95" t="s">
-        <v>396</v>
-      </c>
-      <c r="H95" t="s">
-        <v>399</v>
-      </c>
-      <c r="I95" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
@@ -5041,28 +5029,25 @@
         <v>95</v>
       </c>
       <c r="B96">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C96" t="s">
+        <v>399</v>
+      </c>
+      <c r="D96" t="s">
         <v>400</v>
       </c>
-      <c r="D96" t="s">
+      <c r="F96" t="s">
         <v>401</v>
       </c>
-      <c r="E96" t="s">
+      <c r="G96" t="s">
+        <v>399</v>
+      </c>
+      <c r="H96" t="s">
         <v>402</v>
       </c>
-      <c r="F96" t="s">
-        <v>403</v>
-      </c>
-      <c r="G96" t="s">
-        <v>404</v>
-      </c>
-      <c r="H96" t="s">
-        <v>405</v>
-      </c>
       <c r="I96" t="s">
-        <v>406</v>
+        <v>381</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
@@ -5070,28 +5055,28 @@
         <v>96</v>
       </c>
       <c r="B97">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C97" t="s">
+        <v>403</v>
+      </c>
+      <c r="D97" t="s">
+        <v>404</v>
+      </c>
+      <c r="E97" t="s">
+        <v>405</v>
+      </c>
+      <c r="F97" t="s">
+        <v>406</v>
+      </c>
+      <c r="G97" t="s">
         <v>407</v>
       </c>
-      <c r="D97" t="s">
+      <c r="H97" t="s">
         <v>408</v>
       </c>
-      <c r="E97" t="s">
-        <v>402</v>
-      </c>
-      <c r="F97" t="s">
+      <c r="I97" t="s">
         <v>409</v>
-      </c>
-      <c r="G97" t="s">
-        <v>410</v>
-      </c>
-      <c r="H97" t="s">
-        <v>411</v>
-      </c>
-      <c r="I97" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
@@ -5099,28 +5084,28 @@
         <v>97</v>
       </c>
       <c r="B98">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C98" t="s">
+        <v>410</v>
+      </c>
+      <c r="D98" t="s">
+        <v>411</v>
+      </c>
+      <c r="E98" t="s">
+        <v>405</v>
+      </c>
+      <c r="F98" t="s">
         <v>412</v>
       </c>
-      <c r="D98" t="s">
+      <c r="G98" t="s">
         <v>413</v>
       </c>
-      <c r="E98" t="s">
+      <c r="H98" t="s">
         <v>414</v>
       </c>
-      <c r="F98" t="s">
-        <v>415</v>
-      </c>
-      <c r="G98" t="s">
-        <v>416</v>
-      </c>
-      <c r="H98" t="s">
-        <v>417</v>
-      </c>
       <c r="I98" t="s">
-        <v>418</v>
+        <v>409</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
@@ -5131,25 +5116,25 @@
         <v>1</v>
       </c>
       <c r="C99" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="D99" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E99" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="F99" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="G99" t="s">
         <v>419</v>
       </c>
       <c r="H99" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="I99" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
@@ -5157,28 +5142,28 @@
         <v>99</v>
       </c>
       <c r="B100">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C100" t="s">
+        <v>422</v>
+      </c>
+      <c r="D100" t="s">
+        <v>423</v>
+      </c>
+      <c r="E100" t="s">
+        <v>424</v>
+      </c>
+      <c r="F100" t="s">
         <v>425</v>
       </c>
-      <c r="D100" t="s">
-        <v>401</v>
-      </c>
-      <c r="E100" t="s">
-        <v>402</v>
-      </c>
-      <c r="F100" t="s">
+      <c r="G100" t="s">
+        <v>422</v>
+      </c>
+      <c r="H100" t="s">
         <v>426</v>
       </c>
-      <c r="G100" t="s">
+      <c r="I100" t="s">
         <v>427</v>
-      </c>
-      <c r="H100" t="s">
-        <v>428</v>
-      </c>
-      <c r="I100" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
@@ -5186,28 +5171,28 @@
         <v>100</v>
       </c>
       <c r="B101">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="C101" t="s">
+        <v>428</v>
+      </c>
+      <c r="D101" t="s">
+        <v>404</v>
+      </c>
+      <c r="E101" t="s">
+        <v>405</v>
+      </c>
+      <c r="F101" t="s">
         <v>429</v>
       </c>
-      <c r="D101" t="s">
+      <c r="G101" t="s">
         <v>430</v>
       </c>
-      <c r="E101" t="s">
+      <c r="H101" t="s">
         <v>431</v>
       </c>
-      <c r="F101" t="s">
-        <v>432</v>
-      </c>
-      <c r="G101" t="s">
-        <v>433</v>
-      </c>
-      <c r="H101" t="s">
-        <v>434</v>
-      </c>
       <c r="I101" t="s">
-        <v>435</v>
+        <v>409</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
@@ -5215,28 +5200,28 @@
         <v>101</v>
       </c>
       <c r="B102">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C102" t="s">
+        <v>432</v>
+      </c>
+      <c r="D102" t="s">
+        <v>433</v>
+      </c>
+      <c r="E102" t="s">
+        <v>434</v>
+      </c>
+      <c r="F102" t="s">
+        <v>435</v>
+      </c>
+      <c r="G102" t="s">
         <v>436</v>
       </c>
-      <c r="D102" t="s">
+      <c r="H102" t="s">
         <v>437</v>
       </c>
-      <c r="E102" t="s">
+      <c r="I102" t="s">
         <v>438</v>
-      </c>
-      <c r="F102" t="s">
-        <v>439</v>
-      </c>
-      <c r="G102" t="s">
-        <v>440</v>
-      </c>
-      <c r="H102" t="s">
-        <v>441</v>
-      </c>
-      <c r="I102" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
@@ -5244,28 +5229,28 @@
         <v>102</v>
       </c>
       <c r="B103">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="C103" t="s">
+        <v>439</v>
+      </c>
+      <c r="D103" t="s">
+        <v>440</v>
+      </c>
+      <c r="E103" t="s">
+        <v>441</v>
+      </c>
+      <c r="F103" t="s">
         <v>442</v>
       </c>
-      <c r="D103" t="s">
+      <c r="G103" t="s">
         <v>443</v>
       </c>
-      <c r="E103" t="s">
-        <v>431</v>
-      </c>
-      <c r="F103" t="s">
+      <c r="H103" t="s">
         <v>444</v>
       </c>
-      <c r="G103" t="s">
-        <v>445</v>
-      </c>
-      <c r="H103" t="s">
-        <v>446</v>
-      </c>
       <c r="I103" t="s">
-        <v>395</v>
+        <v>409</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
@@ -5273,28 +5258,28 @@
         <v>103</v>
       </c>
       <c r="B104">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C104" t="s">
+        <v>445</v>
+      </c>
+      <c r="D104" t="s">
+        <v>446</v>
+      </c>
+      <c r="E104" t="s">
+        <v>434</v>
+      </c>
+      <c r="F104" t="s">
         <v>447</v>
       </c>
-      <c r="D104" t="s">
-        <v>401</v>
-      </c>
-      <c r="E104" t="s">
+      <c r="G104" t="s">
         <v>448</v>
       </c>
-      <c r="F104" t="s">
+      <c r="H104" t="s">
         <v>449</v>
       </c>
-      <c r="G104" t="s">
-        <v>427</v>
-      </c>
-      <c r="H104" t="s">
-        <v>450</v>
-      </c>
       <c r="I104" t="s">
-        <v>406</v>
+        <v>398</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
@@ -5302,28 +5287,28 @@
         <v>104</v>
       </c>
       <c r="B105">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C105" t="s">
+        <v>450</v>
+      </c>
+      <c r="D105" t="s">
+        <v>404</v>
+      </c>
+      <c r="E105" t="s">
         <v>451</v>
       </c>
-      <c r="D105" t="s">
+      <c r="F105" t="s">
         <v>452</v>
       </c>
-      <c r="E105" t="s">
+      <c r="G105" t="s">
+        <v>430</v>
+      </c>
+      <c r="H105" t="s">
         <v>453</v>
       </c>
-      <c r="F105" t="s">
-        <v>454</v>
-      </c>
-      <c r="G105" t="s">
-        <v>455</v>
-      </c>
-      <c r="H105" t="s">
-        <v>456</v>
-      </c>
       <c r="I105" t="s">
-        <v>406</v>
+        <v>409</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
@@ -5331,25 +5316,28 @@
         <v>105</v>
       </c>
       <c r="B106">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C106" t="s">
+        <v>454</v>
+      </c>
+      <c r="D106" t="s">
+        <v>455</v>
+      </c>
+      <c r="E106" t="s">
+        <v>456</v>
+      </c>
+      <c r="F106" t="s">
         <v>457</v>
       </c>
-      <c r="D106" t="s">
+      <c r="G106" t="s">
         <v>458</v>
       </c>
-      <c r="F106" t="s">
+      <c r="H106" t="s">
         <v>459</v>
       </c>
-      <c r="G106" t="s">
-        <v>457</v>
-      </c>
-      <c r="H106" t="s">
-        <v>460</v>
-      </c>
       <c r="I106" t="s">
-        <v>461</v>
+        <v>409</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
@@ -5357,25 +5345,25 @@
         <v>106</v>
       </c>
       <c r="B107">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="C107" t="s">
+        <v>460</v>
+      </c>
+      <c r="D107" t="s">
+        <v>461</v>
+      </c>
+      <c r="F107" t="s">
         <v>462</v>
       </c>
-      <c r="D107" t="s">
+      <c r="G107" t="s">
+        <v>460</v>
+      </c>
+      <c r="H107" t="s">
         <v>463</v>
       </c>
-      <c r="F107" t="s">
+      <c r="I107" t="s">
         <v>464</v>
-      </c>
-      <c r="G107" t="s">
-        <v>462</v>
-      </c>
-      <c r="H107" t="s">
-        <v>465</v>
-      </c>
-      <c r="I107" t="s">
-        <v>466</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
@@ -5383,25 +5371,25 @@
         <v>107</v>
       </c>
       <c r="B108">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C108" t="s">
+        <v>465</v>
+      </c>
+      <c r="D108" t="s">
+        <v>466</v>
+      </c>
+      <c r="F108" t="s">
         <v>467</v>
       </c>
-      <c r="D108" t="s">
+      <c r="G108" t="s">
+        <v>465</v>
+      </c>
+      <c r="H108" t="s">
         <v>468</v>
       </c>
-      <c r="F108" t="s">
+      <c r="I108" t="s">
         <v>469</v>
-      </c>
-      <c r="G108" t="s">
-        <v>467</v>
-      </c>
-      <c r="H108" t="s">
-        <v>470</v>
-      </c>
-      <c r="I108" t="s">
-        <v>461</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
@@ -5409,25 +5397,25 @@
         <v>108</v>
       </c>
       <c r="B109">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C109" t="s">
+        <v>470</v>
+      </c>
+      <c r="D109" t="s">
         <v>471</v>
       </c>
-      <c r="D109" t="s">
+      <c r="F109" t="s">
         <v>472</v>
       </c>
-      <c r="F109" t="s">
+      <c r="G109" t="s">
+        <v>470</v>
+      </c>
+      <c r="H109" t="s">
         <v>473</v>
       </c>
-      <c r="G109" t="s">
-        <v>471</v>
-      </c>
-      <c r="H109" t="s">
-        <v>474</v>
-      </c>
       <c r="I109" t="s">
-        <v>461</v>
+        <v>464</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
@@ -5438,22 +5426,22 @@
         <v>1</v>
       </c>
       <c r="C110" t="s">
+        <v>474</v>
+      </c>
+      <c r="D110" t="s">
         <v>475</v>
       </c>
-      <c r="D110" t="s">
+      <c r="F110" t="s">
         <v>476</v>
       </c>
-      <c r="F110" t="s">
+      <c r="G110" t="s">
+        <v>474</v>
+      </c>
+      <c r="H110" t="s">
         <v>477</v>
       </c>
-      <c r="G110" t="s">
-        <v>475</v>
-      </c>
-      <c r="H110" t="s">
-        <v>478</v>
-      </c>
       <c r="I110" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
@@ -5464,25 +5452,22 @@
         <v>1</v>
       </c>
       <c r="C111" t="s">
+        <v>478</v>
+      </c>
+      <c r="D111" t="s">
         <v>479</v>
       </c>
-      <c r="D111" t="s">
+      <c r="F111" t="s">
         <v>480</v>
       </c>
-      <c r="E111" t="s">
+      <c r="G111" t="s">
+        <v>478</v>
+      </c>
+      <c r="H111" t="s">
         <v>481</v>
       </c>
-      <c r="F111" t="s">
-        <v>482</v>
-      </c>
-      <c r="G111" t="s">
-        <v>483</v>
-      </c>
-      <c r="H111" t="s">
-        <v>484</v>
-      </c>
       <c r="I111" t="s">
-        <v>485</v>
+        <v>469</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
@@ -5490,28 +5475,28 @@
         <v>111</v>
       </c>
       <c r="B112">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C112" t="s">
+        <v>482</v>
+      </c>
+      <c r="D112" t="s">
+        <v>483</v>
+      </c>
+      <c r="E112" t="s">
+        <v>484</v>
+      </c>
+      <c r="F112" t="s">
+        <v>485</v>
+      </c>
+      <c r="G112" t="s">
         <v>486</v>
       </c>
-      <c r="D112" t="s">
+      <c r="H112" t="s">
         <v>487</v>
       </c>
-      <c r="E112" t="s">
+      <c r="I112" t="s">
         <v>488</v>
-      </c>
-      <c r="F112" t="s">
-        <v>489</v>
-      </c>
-      <c r="G112" t="s">
-        <v>490</v>
-      </c>
-      <c r="H112" t="s">
-        <v>491</v>
-      </c>
-      <c r="I112" t="s">
-        <v>485</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.25">
@@ -5519,25 +5504,22 @@
         <v>112</v>
       </c>
       <c r="B113">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C113" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="D113" t="s">
-        <v>493</v>
+        <v>490</v>
+      </c>
+      <c r="E113">
+        <v>0</v>
       </c>
       <c r="F113" t="s">
-        <v>494</v>
-      </c>
-      <c r="G113" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="H113" t="s">
-        <v>495</v>
-      </c>
-      <c r="I113" t="s">
-        <v>496</v>
+        <v>489</v>
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
@@ -5548,22 +5530,22 @@
         <v>1</v>
       </c>
       <c r="C114" t="s">
-        <v>497</v>
+        <v>492</v>
       </c>
       <c r="D114" t="s">
-        <v>498</v>
+        <v>493</v>
       </c>
       <c r="F114" t="s">
-        <v>499</v>
+        <v>494</v>
       </c>
       <c r="G114" t="s">
-        <v>497</v>
+        <v>492</v>
       </c>
       <c r="H114" t="s">
-        <v>500</v>
+        <v>495</v>
       </c>
       <c r="I114" t="s">
-        <v>365</v>
+        <v>496</v>
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
@@ -5574,25 +5556,22 @@
         <v>1</v>
       </c>
       <c r="C115" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="D115" t="s">
-        <v>502</v>
-      </c>
-      <c r="E115" t="s">
-        <v>503</v>
+        <v>498</v>
       </c>
       <c r="F115" t="s">
-        <v>504</v>
+        <v>499</v>
       </c>
       <c r="G115" t="s">
-        <v>505</v>
+        <v>497</v>
       </c>
       <c r="H115" t="s">
-        <v>506</v>
+        <v>500</v>
       </c>
       <c r="I115" t="s">
-        <v>507</v>
+        <v>368</v>
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.25">
@@ -5603,22 +5582,22 @@
         <v>1</v>
       </c>
       <c r="C116" t="s">
-        <v>508</v>
+        <v>501</v>
       </c>
       <c r="D116" t="s">
-        <v>509</v>
+        <v>502</v>
       </c>
       <c r="E116" t="s">
-        <v>510</v>
+        <v>503</v>
       </c>
       <c r="F116" t="s">
-        <v>511</v>
+        <v>504</v>
       </c>
       <c r="G116" t="s">
-        <v>512</v>
+        <v>505</v>
       </c>
       <c r="H116" t="s">
-        <v>513</v>
+        <v>506</v>
       </c>
       <c r="I116" t="s">
         <v>507</v>
@@ -5632,22 +5611,22 @@
         <v>1</v>
       </c>
       <c r="C117" t="s">
-        <v>514</v>
+        <v>508</v>
       </c>
       <c r="D117" t="s">
-        <v>515</v>
+        <v>509</v>
       </c>
       <c r="E117" t="s">
-        <v>516</v>
+        <v>510</v>
       </c>
       <c r="F117" t="s">
-        <v>517</v>
+        <v>511</v>
       </c>
       <c r="G117" t="s">
-        <v>518</v>
+        <v>512</v>
       </c>
       <c r="H117" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
       <c r="I117" t="s">
         <v>507</v>
@@ -5661,25 +5640,25 @@
         <v>1</v>
       </c>
       <c r="C118" t="s">
-        <v>520</v>
+        <v>514</v>
       </c>
       <c r="D118" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
       <c r="E118" t="s">
-        <v>522</v>
+        <v>516</v>
       </c>
       <c r="F118" t="s">
-        <v>523</v>
+        <v>517</v>
       </c>
       <c r="G118" t="s">
-        <v>524</v>
+        <v>518</v>
       </c>
       <c r="H118" t="s">
-        <v>525</v>
+        <v>519</v>
       </c>
       <c r="I118" t="s">
-        <v>526</v>
+        <v>507</v>
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.25">
@@ -5690,25 +5669,25 @@
         <v>1</v>
       </c>
       <c r="C119" t="s">
-        <v>527</v>
+        <v>520</v>
       </c>
       <c r="D119" t="s">
-        <v>528</v>
+        <v>521</v>
       </c>
       <c r="E119" t="s">
-        <v>529</v>
+        <v>522</v>
       </c>
       <c r="F119" t="s">
-        <v>530</v>
+        <v>523</v>
       </c>
       <c r="G119" t="s">
-        <v>531</v>
+        <v>524</v>
       </c>
       <c r="H119" t="s">
-        <v>532</v>
+        <v>525</v>
       </c>
       <c r="I119" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.25">
@@ -5719,25 +5698,25 @@
         <v>1</v>
       </c>
       <c r="C120" t="s">
-        <v>534</v>
+        <v>527</v>
       </c>
       <c r="D120" t="s">
-        <v>535</v>
+        <v>528</v>
       </c>
       <c r="E120" t="s">
-        <v>536</v>
+        <v>529</v>
       </c>
       <c r="F120" t="s">
-        <v>537</v>
+        <v>530</v>
       </c>
       <c r="G120" t="s">
-        <v>538</v>
+        <v>531</v>
       </c>
       <c r="H120" t="s">
-        <v>539</v>
+        <v>532</v>
       </c>
       <c r="I120" t="s">
-        <v>540</v>
+        <v>533</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.25">
@@ -5748,25 +5727,25 @@
         <v>1</v>
       </c>
       <c r="C121" t="s">
-        <v>541</v>
+        <v>534</v>
       </c>
       <c r="D121" t="s">
-        <v>542</v>
+        <v>535</v>
       </c>
       <c r="E121" t="s">
-        <v>481</v>
+        <v>536</v>
       </c>
       <c r="F121" t="s">
-        <v>543</v>
+        <v>537</v>
       </c>
       <c r="G121" t="s">
-        <v>512</v>
+        <v>538</v>
       </c>
       <c r="H121" t="s">
-        <v>544</v>
+        <v>539</v>
       </c>
       <c r="I121" t="s">
-        <v>507</v>
+        <v>540</v>
       </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.25">
@@ -5774,25 +5753,28 @@
         <v>121</v>
       </c>
       <c r="B122">
-        <v>94</v>
+        <v>1</v>
       </c>
       <c r="C122" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="D122" t="s">
-        <v>546</v>
-      </c>
-      <c r="E122">
-        <v>0</v>
+        <v>542</v>
+      </c>
+      <c r="E122" t="s">
+        <v>484</v>
       </c>
       <c r="F122" t="s">
-        <v>547</v>
+        <v>543</v>
+      </c>
+      <c r="G122" t="s">
+        <v>512</v>
       </c>
       <c r="H122" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
       <c r="I122" t="s">
-        <v>27</v>
+        <v>507</v>
       </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.25">
@@ -5800,22 +5782,22 @@
         <v>122</v>
       </c>
       <c r="B123">
-        <v>58</v>
+        <v>93</v>
       </c>
       <c r="C123" t="s">
         <v>545</v>
       </c>
       <c r="D123" t="s">
-        <v>549</v>
-      </c>
-      <c r="E123" t="s">
-        <v>550</v>
+        <v>546</v>
+      </c>
+      <c r="E123">
+        <v>0</v>
       </c>
       <c r="F123" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="H123" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
       <c r="I123" t="s">
         <v>27</v>
@@ -5826,7 +5808,7 @@
         <v>123</v>
       </c>
       <c r="B124">
-        <v>22</v>
+        <v>58</v>
       </c>
       <c r="C124" t="s">
         <v>545</v>
@@ -5835,13 +5817,13 @@
         <v>549</v>
       </c>
       <c r="E124" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="F124" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="H124" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="I124" t="s">
         <v>27</v>
@@ -5852,7 +5834,7 @@
         <v>124</v>
       </c>
       <c r="B125">
-        <v>140</v>
+        <v>24</v>
       </c>
       <c r="C125" t="s">
         <v>545</v>
@@ -5861,16 +5843,13 @@
         <v>549</v>
       </c>
       <c r="E125" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="F125" t="s">
-        <v>557</v>
-      </c>
-      <c r="G125" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="H125" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="I125" t="s">
         <v>27</v>
@@ -5881,25 +5860,25 @@
         <v>125</v>
       </c>
       <c r="B126">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C126" t="s">
         <v>545</v>
       </c>
       <c r="D126" t="s">
-        <v>549</v>
-      </c>
-      <c r="E126">
-        <v>100</v>
+        <v>556</v>
+      </c>
+      <c r="E126" t="s">
+        <v>34</v>
       </c>
       <c r="F126" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="H126" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="I126" t="s">
-        <v>27</v>
+        <v>559</v>
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.25">
@@ -5907,7 +5886,7 @@
         <v>126</v>
       </c>
       <c r="B127">
-        <v>11</v>
+        <v>141</v>
       </c>
       <c r="C127" t="s">
         <v>545</v>
@@ -5915,10 +5894,13 @@
       <c r="D127" t="s">
         <v>549</v>
       </c>
-      <c r="E127">
-        <v>330</v>
+      <c r="E127" t="s">
+        <v>560</v>
       </c>
       <c r="F127" t="s">
+        <v>561</v>
+      </c>
+      <c r="G127" t="s">
         <v>562</v>
       </c>
       <c r="H127" t="s">
@@ -5933,7 +5915,7 @@
         <v>127</v>
       </c>
       <c r="B128">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="C128" t="s">
         <v>545</v>
@@ -5941,14 +5923,14 @@
       <c r="D128" t="s">
         <v>549</v>
       </c>
-      <c r="E128" t="s">
+      <c r="E128">
+        <v>100</v>
+      </c>
+      <c r="F128" t="s">
         <v>564</v>
       </c>
-      <c r="F128" t="s">
+      <c r="H128" t="s">
         <v>565</v>
-      </c>
-      <c r="H128" t="s">
-        <v>566</v>
       </c>
       <c r="I128" t="s">
         <v>27</v>
@@ -5959,25 +5941,25 @@
         <v>128</v>
       </c>
       <c r="B129">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C129" t="s">
         <v>545</v>
       </c>
       <c r="D129" t="s">
+        <v>549</v>
+      </c>
+      <c r="E129">
+        <v>330</v>
+      </c>
+      <c r="F129" t="s">
+        <v>566</v>
+      </c>
+      <c r="H129" t="s">
         <v>567</v>
       </c>
-      <c r="E129" t="s">
-        <v>34</v>
-      </c>
-      <c r="F129" t="s">
-        <v>568</v>
-      </c>
-      <c r="H129" t="s">
-        <v>569</v>
-      </c>
       <c r="I129" t="s">
-        <v>570</v>
+        <v>27</v>
       </c>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.25">
@@ -5985,7 +5967,7 @@
         <v>129</v>
       </c>
       <c r="B130">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="C130" t="s">
         <v>545</v>
@@ -5994,13 +5976,13 @@
         <v>549</v>
       </c>
       <c r="E130" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="F130" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="H130" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="I130" t="s">
         <v>27</v>
@@ -6011,7 +5993,7 @@
         <v>130</v>
       </c>
       <c r="B131">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C131" t="s">
         <v>545</v>
@@ -6020,13 +6002,13 @@
         <v>549</v>
       </c>
       <c r="E131" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="F131" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="H131" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="I131" t="s">
         <v>27</v>
@@ -6037,7 +6019,7 @@
         <v>131</v>
       </c>
       <c r="B132">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C132" t="s">
         <v>545</v>
@@ -6046,13 +6028,13 @@
         <v>549</v>
       </c>
       <c r="E132" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="F132" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="H132" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="I132" t="s">
         <v>27</v>
@@ -6063,7 +6045,7 @@
         <v>132</v>
       </c>
       <c r="B133">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C133" t="s">
         <v>545</v>
@@ -6072,13 +6054,13 @@
         <v>549</v>
       </c>
       <c r="E133" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="F133" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="H133" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="I133" t="s">
         <v>27</v>
@@ -6089,7 +6071,7 @@
         <v>133</v>
       </c>
       <c r="B134">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="C134" t="s">
         <v>545</v>
@@ -6097,14 +6079,14 @@
       <c r="D134" t="s">
         <v>549</v>
       </c>
-      <c r="E134">
-        <v>22</v>
+      <c r="E134" t="s">
+        <v>580</v>
       </c>
       <c r="F134" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="H134" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="I134" t="s">
         <v>27</v>
@@ -6115,7 +6097,7 @@
         <v>134</v>
       </c>
       <c r="B135">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="C135" t="s">
         <v>545</v>
@@ -6124,13 +6106,13 @@
         <v>549</v>
       </c>
       <c r="E135">
-        <v>240</v>
+        <v>22</v>
       </c>
       <c r="F135" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="H135" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="I135" t="s">
         <v>27</v>
@@ -6141,7 +6123,7 @@
         <v>135</v>
       </c>
       <c r="B136">
-        <v>75</v>
+        <v>22</v>
       </c>
       <c r="C136" t="s">
         <v>545</v>
@@ -6150,13 +6132,13 @@
         <v>549</v>
       </c>
       <c r="E136">
-        <v>39</v>
+        <v>240</v>
       </c>
       <c r="F136" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="H136" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="I136" t="s">
         <v>27</v>
@@ -6167,7 +6149,7 @@
         <v>136</v>
       </c>
       <c r="B137">
-        <v>5</v>
+        <v>75</v>
       </c>
       <c r="C137" t="s">
         <v>545</v>
@@ -6176,13 +6158,13 @@
         <v>549</v>
       </c>
       <c r="E137">
-        <v>499</v>
+        <v>39</v>
       </c>
       <c r="F137" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="H137" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="I137" t="s">
         <v>27</v>
@@ -6193,7 +6175,7 @@
         <v>137</v>
       </c>
       <c r="B138">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C138" t="s">
         <v>545</v>
@@ -6202,13 +6184,13 @@
         <v>549</v>
       </c>
       <c r="E138">
-        <v>36</v>
+        <v>499</v>
       </c>
       <c r="F138" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="H138" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="I138" t="s">
         <v>27</v>
@@ -6219,7 +6201,7 @@
         <v>138</v>
       </c>
       <c r="B139">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C139" t="s">
         <v>545</v>
@@ -6228,13 +6210,13 @@
         <v>549</v>
       </c>
       <c r="E139">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="F139" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="H139" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="I139" t="s">
         <v>27</v>
@@ -6245,7 +6227,7 @@
         <v>139</v>
       </c>
       <c r="B140">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C140" t="s">
         <v>545</v>
@@ -6253,14 +6235,14 @@
       <c r="D140" t="s">
         <v>549</v>
       </c>
-      <c r="E140" t="s">
-        <v>595</v>
+      <c r="E140">
+        <v>10</v>
       </c>
       <c r="F140" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="H140" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="I140" t="s">
         <v>27</v>
@@ -6280,13 +6262,13 @@
         <v>549</v>
       </c>
       <c r="E141" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="F141" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="H141" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="I141" t="s">
         <v>27</v>
@@ -6297,25 +6279,25 @@
         <v>141</v>
       </c>
       <c r="B142">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="C142" t="s">
         <v>545</v>
       </c>
       <c r="D142" t="s">
-        <v>601</v>
+        <v>549</v>
       </c>
       <c r="E142" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
       <c r="F142" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="H142" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="I142" t="s">
-        <v>602</v>
+        <v>27</v>
       </c>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.25">
@@ -6323,25 +6305,25 @@
         <v>142</v>
       </c>
       <c r="B143">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="C143" t="s">
-        <v>605</v>
+        <v>545</v>
       </c>
       <c r="D143" t="s">
-        <v>606</v>
+        <v>601</v>
       </c>
       <c r="E143" t="s">
-        <v>595</v>
+        <v>602</v>
       </c>
       <c r="F143" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="H143" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
       <c r="I143" t="s">
-        <v>27</v>
+        <v>602</v>
       </c>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.25">
@@ -6349,22 +6331,22 @@
         <v>143</v>
       </c>
       <c r="B144">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C144" t="s">
-        <v>609</v>
+        <v>605</v>
       </c>
       <c r="D144" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
       <c r="E144" t="s">
-        <v>611</v>
+        <v>595</v>
       </c>
       <c r="F144" t="s">
-        <v>612</v>
+        <v>607</v>
       </c>
       <c r="H144" t="s">
-        <v>613</v>
+        <v>608</v>
       </c>
       <c r="I144" t="s">
         <v>27</v>
@@ -6375,7 +6357,7 @@
         <v>144</v>
       </c>
       <c r="B145">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C145" t="s">
         <v>609</v>
@@ -6384,13 +6366,13 @@
         <v>610</v>
       </c>
       <c r="E145" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="F145" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="H145" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="I145" t="s">
         <v>27</v>
@@ -6401,25 +6383,25 @@
         <v>145</v>
       </c>
       <c r="B146">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C146" t="s">
-        <v>617</v>
+        <v>609</v>
       </c>
       <c r="D146" t="s">
-        <v>618</v>
+        <v>610</v>
       </c>
       <c r="E146" t="s">
-        <v>602</v>
+        <v>614</v>
       </c>
       <c r="F146" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
       <c r="H146" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
       <c r="I146" t="s">
-        <v>602</v>
+        <v>27</v>
       </c>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.25">
@@ -6430,22 +6412,22 @@
         <v>2</v>
       </c>
       <c r="C147" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="D147" t="s">
-        <v>622</v>
+        <v>618</v>
       </c>
       <c r="E147" t="s">
-        <v>623</v>
+        <v>602</v>
       </c>
       <c r="F147" t="s">
-        <v>624</v>
+        <v>619</v>
       </c>
       <c r="H147" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="I147" t="s">
-        <v>626</v>
+        <v>602</v>
       </c>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.25">
@@ -6453,25 +6435,25 @@
         <v>147</v>
       </c>
       <c r="B148">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C148" t="s">
-        <v>627</v>
+        <v>621</v>
       </c>
       <c r="D148" t="s">
-        <v>628</v>
+        <v>622</v>
       </c>
       <c r="E148" t="s">
         <v>623</v>
       </c>
       <c r="F148" t="s">
-        <v>629</v>
+        <v>624</v>
       </c>
       <c r="H148" t="s">
-        <v>630</v>
+        <v>625</v>
       </c>
       <c r="I148" t="s">
-        <v>631</v>
+        <v>626</v>
       </c>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.25">
@@ -6482,7 +6464,7 @@
         <v>15</v>
       </c>
       <c r="C149" t="s">
-        <v>632</v>
+        <v>627</v>
       </c>
       <c r="D149" t="s">
         <v>606</v>
@@ -6491,10 +6473,10 @@
         <v>100</v>
       </c>
       <c r="F149" t="s">
-        <v>633</v>
+        <v>628</v>
       </c>
       <c r="H149" t="s">
-        <v>634</v>
+        <v>629</v>
       </c>
       <c r="I149" t="s">
         <v>27</v>
@@ -6508,19 +6490,19 @@
         <v>1</v>
       </c>
       <c r="C150" t="s">
-        <v>635</v>
+        <v>630</v>
       </c>
       <c r="D150" t="s">
         <v>549</v>
       </c>
       <c r="E150" t="s">
-        <v>636</v>
+        <v>631</v>
       </c>
       <c r="F150" t="s">
-        <v>637</v>
+        <v>632</v>
       </c>
       <c r="H150" t="s">
-        <v>638</v>
+        <v>633</v>
       </c>
       <c r="I150" t="s">
         <v>27</v>
@@ -6540,16 +6522,16 @@
         <v>549</v>
       </c>
       <c r="E151" t="s">
-        <v>639</v>
+        <v>634</v>
       </c>
       <c r="F151" t="s">
-        <v>640</v>
+        <v>635</v>
       </c>
       <c r="G151" t="s">
-        <v>558</v>
+        <v>562</v>
       </c>
       <c r="H151" t="s">
-        <v>641</v>
+        <v>636</v>
       </c>
       <c r="I151" t="s">
         <v>27</v>
@@ -6572,10 +6554,10 @@
         <v>33</v>
       </c>
       <c r="F152" t="s">
-        <v>642</v>
+        <v>637</v>
       </c>
       <c r="H152" t="s">
-        <v>643</v>
+        <v>638</v>
       </c>
       <c r="I152" t="s">
         <v>27</v>
@@ -6586,22 +6568,22 @@
         <v>152</v>
       </c>
       <c r="B153">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C153" t="s">
-        <v>644</v>
+        <v>639</v>
       </c>
       <c r="D153" t="s">
-        <v>645</v>
+        <v>640</v>
       </c>
       <c r="E153">
         <v>0</v>
       </c>
       <c r="F153" t="s">
-        <v>646</v>
+        <v>641</v>
       </c>
       <c r="H153" t="s">
-        <v>647</v>
+        <v>642</v>
       </c>
       <c r="I153" t="s">
         <v>27</v>
@@ -6621,13 +6603,13 @@
         <v>549</v>
       </c>
       <c r="E154" t="s">
-        <v>648</v>
+        <v>643</v>
       </c>
       <c r="F154" t="s">
-        <v>649</v>
+        <v>644</v>
       </c>
       <c r="H154" t="s">
-        <v>650</v>
+        <v>645</v>
       </c>
       <c r="I154" t="s">
         <v>27</v>
@@ -6647,13 +6629,13 @@
         <v>549</v>
       </c>
       <c r="E155" t="s">
-        <v>651</v>
+        <v>646</v>
       </c>
       <c r="F155" t="s">
-        <v>652</v>
+        <v>647</v>
       </c>
       <c r="H155" t="s">
-        <v>653</v>
+        <v>648</v>
       </c>
       <c r="I155" t="s">
         <v>27</v>
@@ -6667,22 +6649,22 @@
         <v>1</v>
       </c>
       <c r="C156" t="s">
-        <v>654</v>
+        <v>649</v>
       </c>
       <c r="D156" t="s">
-        <v>655</v>
+        <v>606</v>
+      </c>
+      <c r="E156" t="s">
+        <v>650</v>
       </c>
       <c r="F156" t="s">
-        <v>656</v>
-      </c>
-      <c r="G156" t="s">
-        <v>654</v>
+        <v>651</v>
       </c>
       <c r="H156" t="s">
-        <v>657</v>
+        <v>652</v>
       </c>
       <c r="I156" t="s">
-        <v>658</v>
+        <v>27</v>
       </c>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.25">
@@ -6693,22 +6675,22 @@
         <v>2</v>
       </c>
       <c r="C157" t="s">
-        <v>659</v>
+        <v>653</v>
       </c>
       <c r="D157" t="s">
-        <v>660</v>
+        <v>654</v>
       </c>
       <c r="F157" t="s">
-        <v>661</v>
+        <v>655</v>
       </c>
       <c r="G157" t="s">
-        <v>659</v>
+        <v>653</v>
       </c>
       <c r="H157" t="s">
-        <v>662</v>
+        <v>656</v>
       </c>
       <c r="I157" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.25">
@@ -6719,22 +6701,22 @@
         <v>10</v>
       </c>
       <c r="C158" t="s">
-        <v>663</v>
+        <v>658</v>
       </c>
       <c r="D158" t="s">
-        <v>664</v>
+        <v>659</v>
       </c>
       <c r="F158" t="s">
-        <v>665</v>
+        <v>660</v>
       </c>
       <c r="G158" t="s">
-        <v>666</v>
+        <v>661</v>
       </c>
       <c r="H158" t="s">
-        <v>663</v>
+        <v>658</v>
       </c>
       <c r="I158" t="s">
-        <v>667</v>
+        <v>662</v>
       </c>
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.25">
@@ -6745,22 +6727,22 @@
         <v>2</v>
       </c>
       <c r="C159" t="s">
-        <v>668</v>
+        <v>663</v>
       </c>
       <c r="D159" t="s">
-        <v>669</v>
+        <v>664</v>
       </c>
       <c r="F159" t="s">
-        <v>670</v>
+        <v>665</v>
       </c>
       <c r="G159" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="H159" t="s">
-        <v>668</v>
+        <v>663</v>
       </c>
       <c r="I159" t="s">
-        <v>671</v>
+        <v>666</v>
       </c>
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.25">
@@ -6771,19 +6753,19 @@
         <v>6</v>
       </c>
       <c r="C160" t="s">
-        <v>672</v>
+        <v>667</v>
       </c>
       <c r="D160" t="s">
-        <v>673</v>
+        <v>668</v>
       </c>
       <c r="F160" t="s">
-        <v>674</v>
+        <v>669</v>
       </c>
       <c r="G160" t="s">
-        <v>675</v>
+        <v>670</v>
       </c>
       <c r="H160" t="s">
-        <v>672</v>
+        <v>667</v>
       </c>
       <c r="I160" t="s">
         <v>149</v>
@@ -6794,25 +6776,25 @@
         <v>160</v>
       </c>
       <c r="B161">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C161" t="s">
-        <v>676</v>
+        <v>671</v>
       </c>
       <c r="D161" t="s">
-        <v>677</v>
+        <v>672</v>
       </c>
       <c r="F161" t="s">
-        <v>678</v>
+        <v>673</v>
       </c>
       <c r="G161" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="H161" t="s">
-        <v>676</v>
+        <v>671</v>
       </c>
       <c r="I161" t="s">
-        <v>671</v>
+        <v>666</v>
       </c>
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.25">
@@ -6823,19 +6805,19 @@
         <v>2</v>
       </c>
       <c r="C162" t="s">
-        <v>679</v>
+        <v>674</v>
       </c>
       <c r="D162" t="s">
-        <v>680</v>
+        <v>675</v>
       </c>
       <c r="F162" t="s">
-        <v>681</v>
+        <v>676</v>
       </c>
       <c r="G162" t="s">
-        <v>682</v>
+        <v>677</v>
       </c>
       <c r="H162" t="s">
-        <v>679</v>
+        <v>674</v>
       </c>
       <c r="I162" t="s">
         <v>149</v>
@@ -6849,22 +6831,22 @@
         <v>1</v>
       </c>
       <c r="C163" t="s">
-        <v>683</v>
+        <v>678</v>
       </c>
       <c r="D163" t="s">
-        <v>684</v>
+        <v>679</v>
       </c>
       <c r="F163" t="s">
-        <v>685</v>
+        <v>680</v>
       </c>
       <c r="G163" t="s">
-        <v>686</v>
+        <v>681</v>
       </c>
       <c r="H163" t="s">
-        <v>683</v>
+        <v>678</v>
       </c>
       <c r="I163" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
     </row>
     <row r="164" spans="1:9" x14ac:dyDescent="0.25">
@@ -6875,19 +6857,19 @@
         <v>5</v>
       </c>
       <c r="C164" t="s">
-        <v>687</v>
+        <v>682</v>
       </c>
       <c r="D164" t="s">
-        <v>688</v>
+        <v>683</v>
       </c>
       <c r="F164" t="s">
-        <v>689</v>
+        <v>684</v>
       </c>
       <c r="G164" t="s">
+        <v>677</v>
+      </c>
+      <c r="H164" t="s">
         <v>682</v>
-      </c>
-      <c r="H164" t="s">
-        <v>687</v>
       </c>
       <c r="I164" t="s">
         <v>149</v>
@@ -6901,22 +6883,22 @@
         <v>7</v>
       </c>
       <c r="C165" t="s">
-        <v>690</v>
+        <v>685</v>
       </c>
       <c r="D165" t="s">
-        <v>691</v>
+        <v>686</v>
       </c>
       <c r="F165" t="s">
-        <v>692</v>
+        <v>687</v>
       </c>
       <c r="G165" t="s">
-        <v>693</v>
+        <v>688</v>
       </c>
       <c r="H165" t="s">
-        <v>690</v>
+        <v>685</v>
       </c>
       <c r="I165" t="s">
-        <v>694</v>
+        <v>689</v>
       </c>
     </row>
     <row r="166" spans="1:9" x14ac:dyDescent="0.25">
@@ -6927,19 +6909,19 @@
         <v>1</v>
       </c>
       <c r="C166" t="s">
-        <v>695</v>
+        <v>690</v>
       </c>
       <c r="D166" t="s">
-        <v>696</v>
+        <v>691</v>
       </c>
       <c r="F166" t="s">
-        <v>697</v>
+        <v>692</v>
       </c>
       <c r="G166" t="s">
-        <v>698</v>
+        <v>693</v>
       </c>
       <c r="H166" t="s">
-        <v>695</v>
+        <v>690</v>
       </c>
       <c r="I166" t="s">
         <v>144</v>
@@ -6953,22 +6935,22 @@
         <v>2</v>
       </c>
       <c r="C167" t="s">
-        <v>699</v>
+        <v>694</v>
       </c>
       <c r="D167" t="s">
-        <v>700</v>
+        <v>695</v>
       </c>
       <c r="F167" t="s">
-        <v>701</v>
+        <v>696</v>
       </c>
       <c r="G167" t="s">
-        <v>699</v>
+        <v>694</v>
       </c>
       <c r="H167" t="s">
-        <v>702</v>
+        <v>697</v>
       </c>
       <c r="I167" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
     </row>
     <row r="168" spans="1:9" x14ac:dyDescent="0.25">
@@ -6979,25 +6961,25 @@
         <v>2</v>
       </c>
       <c r="C168" t="s">
+        <v>698</v>
+      </c>
+      <c r="D168" t="s">
+        <v>699</v>
+      </c>
+      <c r="E168" t="s">
+        <v>700</v>
+      </c>
+      <c r="F168" t="s">
+        <v>701</v>
+      </c>
+      <c r="G168" t="s">
+        <v>702</v>
+      </c>
+      <c r="H168" t="s">
         <v>703</v>
       </c>
-      <c r="D168" t="s">
-        <v>704</v>
-      </c>
-      <c r="E168" t="s">
-        <v>705</v>
-      </c>
-      <c r="F168" t="s">
-        <v>706</v>
-      </c>
-      <c r="G168" t="s">
-        <v>707</v>
-      </c>
-      <c r="H168" t="s">
-        <v>708</v>
-      </c>
       <c r="I168" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
     </row>
     <row r="169" spans="1:9" x14ac:dyDescent="0.25">
@@ -7008,22 +6990,22 @@
         <v>3</v>
       </c>
       <c r="C169" t="s">
-        <v>709</v>
+        <v>704</v>
       </c>
       <c r="D169" t="s">
-        <v>710</v>
+        <v>705</v>
       </c>
       <c r="F169" t="s">
-        <v>711</v>
+        <v>706</v>
       </c>
       <c r="G169" t="s">
-        <v>709</v>
+        <v>704</v>
       </c>
       <c r="H169" t="s">
-        <v>712</v>
+        <v>707</v>
       </c>
       <c r="I169" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
     </row>
   </sheetData>

</xml_diff>